<commit_message>
Correction on heat sector data (1)
</commit_message>
<xml_diff>
--- a/Inputs/JRC_EU_TIMES/NearZeroCarbon/TIMES_DH_Demand_2050.xlsx
+++ b/Inputs/JRC_EU_TIMES/NearZeroCarbon/TIMES_DH_Demand_2050.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\DispaSET-SideTools\Inputs\JRC_EU_TIMES\NearZeroCarbon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18675533-6FCF-4460-A690-E85B22AB4F6A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{21A576B3-8052-40DC-8844-871038547424}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6683F21A-AB33-434C-ADE1-7B016C840456}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0CA47C51-E4EF-4A12-89C5-9ED7FBDB7BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Region</t>
-  </si>
-  <si>
-    <t>District heat</t>
   </si>
   <si>
     <t>AT</t>
@@ -139,6 +136,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,19 +180,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -510,280 +504,276 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C95591C-8E0D-40CC-9098-ABF0A0EFD49B}">
-  <dimension ref="A1:B33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1C42F5-7602-4C5B-ADBF-D42FFACF7B98}">
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>58.931000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>63.597000000000001</v>
+        <v>17.943000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>17.943000000000001</v>
+        <v>16.956</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>28.100999999999999</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>14.878</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>23.936</v>
+        <v>95.849000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>96.430999999999997</v>
+        <v>473.41200000000003</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>475.73900000000003</v>
+        <v>42.966999999999992</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>98.954999999999998</v>
+        <v>17.175000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>20.516000000000002</v>
+        <v>0.17499999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>4.5279999999999996</v>
+        <v>7.0380000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>29.311</v>
+        <v>48.101999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>129.697</v>
+        <v>24.015000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>1113.008</v>
+        <v>9.1750000000000007</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>9.1750000000000007</v>
+        <v>35.707999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>35.707999999999998</v>
+        <v>0.92100000000000004</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>0.92100000000000004</v>
+        <v>9.9589999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>9.9589999999999996</v>
+        <v>249.614</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>669.39499999999998</v>
+        <v>29.657</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>31.718</v>
+        <v>0.93800000000000006</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>1.639</v>
+        <v>21.543000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>21.543000000000003</v>
+        <v>0.31900000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>0.36499999999999999</v>
+        <v>63.656000000000006</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>138.87400000000002</v>
+        <v>25.529</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>31.436</v>
+        <v>189.928</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>201.642</v>
+        <v>13.797000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>326.78400000000005</v>
+        <v>108.97500000000001</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>108.97500000000001</v>
+        <v>110.334</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>520.12800000000004</v>
+        <v>6.6379999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>7.4350000000000005</v>
+        <v>24.414000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>29.376000000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1">
-        <v>39.734999999999999</v>
+        <v>21.408999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>